<commit_message>
wijzigingen om de boel wat beter vorm te geven.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart/Sites/timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4721C9FD-6523-7F4C-8082-C46439DB246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3D707-8CA2-1148-8438-0FB1CF141F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{6F048ECD-FB1E-5E47-8340-0B45BC6D7F7B}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="1" xr2:uid="{6F048ECD-FB1E-5E47-8340-0B45BC6D7F7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="swimlanes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="127">
   <si>
     <t>Leon Battista Alberti</t>
   </si>
@@ -796,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDA60B0-880A-B248-A4AA-06811654C0F6}">
   <dimension ref="B3:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1264,4 +1265,457 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8F1AE0-6983-804C-A425-9516D43EA6BD}">
+  <dimension ref="B3:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E18" r:id="rId1" xr:uid="{75FE1603-6372-904E-B51F-6631721816A0}"/>
+    <hyperlink ref="E23" r:id="rId2" xr:uid="{2890505F-0BF9-2141-87A9-B1FBA40053BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Medici toegevoegd; die timeline code behoorlijk uitgeplozen en gerefactord.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart/Sites/timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3D707-8CA2-1148-8438-0FB1CF141F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580B1CF-3F69-8341-BDA2-AC4E8A626D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="1" xr2:uid="{6F048ECD-FB1E-5E47-8340-0B45BC6D7F7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="swimlanes" sheetId="2" r:id="rId2"/>
+    <sheet name="artists" sheetId="1" r:id="rId1"/>
+    <sheet name="medici" sheetId="3" r:id="rId2"/>
+    <sheet name="events" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="170">
   <si>
     <t>Leon Battista Alberti</t>
   </si>
@@ -106,9 +107,6 @@
     <t>Artiesten</t>
   </si>
   <si>
-    <t>Naam</t>
-  </si>
-  <si>
     <t>van</t>
   </si>
   <si>
@@ -416,6 +414,138 @@
   </si>
   <si>
     <t xml:space="preserve">Medici </t>
+  </si>
+  <si>
+    <t>naam</t>
+  </si>
+  <si>
+    <t>Gutenberg Bible</t>
+  </si>
+  <si>
+    <t>moment</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Gutenberg_Bible</t>
+  </si>
+  <si>
+    <t>1453-10-19</t>
+  </si>
+  <si>
+    <t>End of hundred year's war</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Guerra_dei_cent%27anni</t>
+  </si>
+  <si>
+    <t>Medici</t>
+  </si>
+  <si>
+    <t>Alessandro de' Medici</t>
+  </si>
+  <si>
+    <t>Caterina de'Medici</t>
+  </si>
+  <si>
+    <t>Cosimo de' Medici</t>
+  </si>
+  <si>
+    <t>Francesco de' Medici</t>
+  </si>
+  <si>
+    <t>Giovanni de'Medici</t>
+  </si>
+  <si>
+    <t>Giulio de'Medici</t>
+  </si>
+  <si>
+    <t>Ippolito de'Medici</t>
+  </si>
+  <si>
+    <t>Lorenzo de'Medici</t>
+  </si>
+  <si>
+    <t>Ottaviano de'Medici</t>
+  </si>
+  <si>
+    <t>1510-07-22</t>
+  </si>
+  <si>
+    <t>1537-01-06</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Alessandro_de%27_Medici_(duca_di_Firenze)</t>
+  </si>
+  <si>
+    <t>1518-04-13</t>
+  </si>
+  <si>
+    <t>1589-01-05</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Caterina_de%27_Medici</t>
+  </si>
+  <si>
+    <t>1389-09-27</t>
+  </si>
+  <si>
+    <t>1464-08-01</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Cosimo_de%27_Medici</t>
+  </si>
+  <si>
+    <t>1541-03-25</t>
+  </si>
+  <si>
+    <t>1587-10-19</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Francesco_I_de%27_Medici</t>
+  </si>
+  <si>
+    <t>1475-12-11</t>
+  </si>
+  <si>
+    <t>1521-12-01</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Papa_Leone_X</t>
+  </si>
+  <si>
+    <t>1478-05-26</t>
+  </si>
+  <si>
+    <t>1534-09-25</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Papa_Clemente_VII</t>
+  </si>
+  <si>
+    <t>1511-03-01</t>
+  </si>
+  <si>
+    <t>1535-10-10</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Ippolito_de%27_Medici</t>
+  </si>
+  <si>
+    <t>1449-01-01</t>
+  </si>
+  <si>
+    <t>1492-04-08</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Lorenzo_de%27_Medici</t>
+  </si>
+  <si>
+    <t>1484-07-14</t>
+  </si>
+  <si>
+    <t>1546-05-28</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Ottaviano_de%27_Medici</t>
   </si>
 </sst>
 </file>
@@ -798,7 +928,7 @@
   <dimension ref="B3:E38"/>
   <sheetViews>
     <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E34"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,16 +946,16 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -833,13 +963,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -847,13 +977,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -861,13 +991,13 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -875,13 +1005,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -889,27 +1019,27 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -917,13 +1047,13 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -931,13 +1061,13 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -945,27 +1075,27 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>53</v>
-      </c>
-      <c r="E13" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -973,13 +1103,13 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -987,27 +1117,27 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
         <v>65</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>67</v>
-      </c>
-      <c r="E17" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
@@ -1015,13 +1145,13 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
         <v>69</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>70</v>
-      </c>
-      <c r="E18" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -1029,13 +1159,13 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -1043,13 +1173,13 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
         <v>75</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>76</v>
-      </c>
-      <c r="E20" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -1057,27 +1187,27 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="s">
         <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" t="s">
         <v>81</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
@@ -1085,13 +1215,13 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
         <v>85</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
@@ -1099,13 +1229,13 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" t="s">
         <v>88</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
@@ -1113,13 +1243,13 @@
         <v>16</v>
       </c>
       <c r="C25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
         <v>91</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>92</v>
-      </c>
-      <c r="E25" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
@@ -1127,27 +1257,27 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
         <v>94</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>95</v>
-      </c>
-      <c r="E26" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
         <v>97</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>98</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>99</v>
-      </c>
-      <c r="E27" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
@@ -1155,27 +1285,27 @@
         <v>18</v>
       </c>
       <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" t="s">
         <v>101</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>102</v>
-      </c>
-      <c r="E28" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s">
         <v>104</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>105</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>106</v>
-      </c>
-      <c r="E29" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
@@ -1183,13 +1313,13 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
         <v>108</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>109</v>
-      </c>
-      <c r="E30" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
@@ -1197,13 +1327,13 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
         <v>111</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>112</v>
-      </c>
-      <c r="E31" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
@@ -1211,51 +1341,51 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
         <v>114</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>115</v>
-      </c>
-      <c r="E32" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" t="s">
         <v>117</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" t="s">
         <v>118</v>
-      </c>
-      <c r="D33" t="s">
-        <v>120</v>
-      </c>
-      <c r="E33" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" t="s">
         <v>121</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>122</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>123</v>
-      </c>
-      <c r="E34" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1268,454 +1398,224 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BD704F-AF10-9E4B-A632-511F1E973F6C}">
+  <dimension ref="B3:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{0D5DF9EC-C502-1249-93E4-8D2CD3E6F8A7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8F1AE0-6983-804C-A425-9516D43EA6BD}">
-  <dimension ref="B3:E33"/>
+  <dimension ref="B3:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>128</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
+        <v>127</v>
+      </c>
+      <c r="C4">
+        <v>1450</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" t="s">
-        <v>115</v>
-      </c>
-      <c r="E31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
-      </c>
-      <c r="E32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" t="s">
-        <v>124</v>
-      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1" xr:uid="{75FE1603-6372-904E-B51F-6631721816A0}"/>
-    <hyperlink ref="E23" r:id="rId2" xr:uid="{2890505F-0BF9-2141-87A9-B1FBA40053BD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added events; major refactoring of the given code.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart/Sites/timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580B1CF-3F69-8341-BDA2-AC4E8A626D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B15B0D6-C2D5-0A49-B677-72EC5C19E364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="1" xr2:uid="{6F048ECD-FB1E-5E47-8340-0B45BC6D7F7B}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="2" xr2:uid="{6F048ECD-FB1E-5E47-8340-0B45BC6D7F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="artists" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="197">
   <si>
     <t>Leon Battista Alberti</t>
   </si>
@@ -546,6 +544,87 @@
   </si>
   <si>
     <t>https://it.wikipedia.org/wiki/Ottaviano_de%27_Medici</t>
+  </si>
+  <si>
+    <t>Coronation of Charles V</t>
+  </si>
+  <si>
+    <t>Sack of Rome</t>
+  </si>
+  <si>
+    <t>Finding of Laocoön</t>
+  </si>
+  <si>
+    <t>Battle of Cascina</t>
+  </si>
+  <si>
+    <t>Council of Trent</t>
+  </si>
+  <si>
+    <t>St. Bartholomew's Massacre</t>
+  </si>
+  <si>
+    <t>Battle of Anghiari</t>
+  </si>
+  <si>
+    <t>Opening of Uffizi</t>
+  </si>
+  <si>
+    <t>Opening of Accademia di belle arti</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Accademia_delle_arti_del_disegno</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Coronation_of_Charles_V</t>
+  </si>
+  <si>
+    <t>1530-02-24</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Sacco_di_Roma_(1527)</t>
+  </si>
+  <si>
+    <t>1527-05-06</t>
+  </si>
+  <si>
+    <t>1506-01-15</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Gruppo_del_Laocoonte#Il_ritrovamento</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Battaglia_di_Cascina</t>
+  </si>
+  <si>
+    <t>1364-07-13</t>
+  </si>
+  <si>
+    <t>Edict of Worms</t>
+  </si>
+  <si>
+    <t>1521-05-25</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Diet_of_Worms#Edict_of_Worms</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Council_of_Trent</t>
+  </si>
+  <si>
+    <t>1572-08-24</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/St._Bartholomew%27s_Day_massacre</t>
+  </si>
+  <si>
+    <t>1440-06-29</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Battle_of_Anghiari</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Uffizi</t>
   </si>
 </sst>
 </file>
@@ -612,7 +691,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -629,7 +708,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1401,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BD704F-AF10-9E4B-A632-511F1E973F6C}">
   <dimension ref="B3:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="164" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1431,86 +1510,86 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="E9" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" t="s">
-        <v>160</v>
+        <v>144</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -1529,35 +1608,38 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="E13" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E13">
+    <sortCondition ref="C5:C13"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{0D5DF9EC-C502-1249-93E4-8D2CD3E6F8A7}"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{0D5DF9EC-C502-1249-93E4-8D2CD3E6F8A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1567,11 +1649,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8F1AE0-6983-804C-A425-9516D43EA6BD}">
   <dimension ref="B3:E23"/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -1606,7 +1691,115 @@
         <v>132</v>
       </c>
     </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6">
+        <v>1563</v>
+      </c>
+      <c r="D6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12">
+        <v>1563</v>
+      </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" t="s">
+        <v>195</v>
+      </c>
+    </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15">
+        <v>1581</v>
+      </c>
+      <c r="D15" t="s">
+        <v>196</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Italiaans verbeterd dankzij Nicole Veronesi.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bart/Sites/timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B15B0D6-C2D5-0A49-B677-72EC5C19E364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF23DDAF-52BF-BF4A-8305-7AB65717B08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="2" xr2:uid="{6F048ECD-FB1E-5E47-8340-0B45BC6D7F7B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="197">
   <si>
     <t>Leon Battista Alberti</t>
   </si>
@@ -420,9 +420,6 @@
     <t>Gutenberg Bible</t>
   </si>
   <si>
-    <t>moment</t>
-  </si>
-  <si>
     <t>https://en.wikipedia.org/wiki/Gutenberg_Bible</t>
   </si>
   <si>
@@ -625,6 +622,9 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Uffizi</t>
+  </si>
+  <si>
+    <t>icon</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1491,7 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -1510,128 +1510,128 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
         <v>149</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>150</v>
-      </c>
-      <c r="E5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
         <v>164</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>165</v>
-      </c>
-      <c r="E6" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
         <v>155</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>156</v>
-      </c>
-      <c r="E7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" t="s">
         <v>158</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>159</v>
-      </c>
-      <c r="E8" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" t="s">
         <v>167</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>168</v>
-      </c>
-      <c r="E9" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" t="s">
         <v>143</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" t="s">
         <v>161</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>162</v>
-      </c>
-      <c r="E11" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" t="s">
         <v>146</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>147</v>
-      </c>
-      <c r="E12" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" t="s">
         <v>152</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>153</v>
-      </c>
-      <c r="E13" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1647,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8F1AE0-6983-804C-A425-9516D43EA6BD}">
-  <dimension ref="B3:E23"/>
+  <dimension ref="B3:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1658,155 +1658,197 @@
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>127</v>
       </c>
       <c r="C4">
         <v>1450</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>1450</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" t="s">
         <v>131</v>
       </c>
-      <c r="C5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C6">
         <v>1563</v>
       </c>
-      <c r="D6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1563</v>
+      </c>
+      <c r="E6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D7" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D8" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>172</v>
       </c>
-      <c r="C9" t="s">
-        <v>184</v>
-      </c>
-      <c r="D9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>173</v>
-      </c>
       <c r="C10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" t="s">
         <v>188</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11" t="s">
         <v>189</v>
       </c>
-      <c r="D11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12">
         <v>1563</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>1563</v>
+      </c>
+      <c r="E12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>175</v>
       </c>
-      <c r="C13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C14" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="D14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>176</v>
-      </c>
-      <c r="C14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>177</v>
       </c>
       <c r="C15">
         <v>1581</v>
       </c>
-      <c r="D15" t="s">
-        <v>196</v>
-      </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E23" s="2"/>
+      <c r="D15">
+        <v>1581</v>
+      </c>
+      <c r="E15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>